<commit_message>
Checklist for the final build
</commit_message>
<xml_diff>
--- a/HEMSv1.1 Configs/Version control.xlsx
+++ b/HEMSv1.1 Configs/Version control.xlsx
@@ -9,19 +9,16 @@
   <sheets>
     <sheet name="Changes" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
   <si>
     <t>Powerloss/Restore logic for all assets</t>
   </si>
   <si>
-    <t>Put additional alert of Asset shutdown alert</t>
-  </si>
-  <si>
     <t>Make sure the features doc has ignition dependancy on RPM by default</t>
   </si>
   <si>
@@ -31,9 +28,6 @@
     <t>Recheck fault detection counter in feature doc</t>
   </si>
   <si>
-    <t>Recheck fualt detection register mapping in feature doc</t>
-  </si>
-  <si>
     <t>Add sec timer for all increment filter</t>
   </si>
   <si>
@@ -47,6 +41,87 @@
   </si>
   <si>
     <t>n/a</t>
+  </si>
+  <si>
+    <t>Pumps</t>
+  </si>
+  <si>
+    <t>Sleep mode end event</t>
+  </si>
+  <si>
+    <t>change fault register from state to event</t>
+  </si>
+  <si>
+    <t>Time inactive filter in IDLS</t>
+  </si>
+  <si>
+    <t>Increase distance from 20 to 50</t>
+  </si>
+  <si>
+    <t>Add GPS validity on geofence</t>
+  </si>
+  <si>
+    <t>Remove geofences</t>
+  </si>
+  <si>
+    <t>Motion based IDLE</t>
+  </si>
+  <si>
+    <t>Access platforms error code will be always FFFFFF</t>
+  </si>
+  <si>
+    <t>Recheck fualt detection register mapping</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>DAP</t>
+  </si>
+  <si>
+    <t>EAP</t>
+  </si>
+  <si>
+    <t>Machinery</t>
+  </si>
+  <si>
+    <t>no alarm lines</t>
+  </si>
+  <si>
+    <t>Generator</t>
+  </si>
+  <si>
+    <t>Add filter on asset shutdown to only send it once</t>
+  </si>
+  <si>
+    <t>FMI form state to event</t>
+  </si>
+  <si>
+    <t>Air Compressor</t>
+  </si>
+  <si>
+    <t>Timer inactive filter for Remote start and stop</t>
+  </si>
+  <si>
+    <t>Operational time</t>
+  </si>
+  <si>
+    <t>Asset features to have macros and customer specific details</t>
+  </si>
+  <si>
+    <t>Put additional filter of Asset shutdown alert</t>
+  </si>
+  <si>
+    <t>Update the changes on version</t>
+  </si>
+  <si>
+    <t>Github update</t>
+  </si>
+  <si>
+    <t>Battery charging start/end after powerup</t>
+  </si>
+  <si>
+    <t>Remove Power disconnect</t>
   </si>
 </sst>
 </file>
@@ -82,8 +157,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -388,92 +466,700 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="65.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="1"/>
+    <col min="4" max="4" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="4.42578125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="B2" s="1">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1">
+        <v>1</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="1">
+        <v>1</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" s="1">
+        <v>1</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="1">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1">
+        <v>1</v>
+      </c>
+      <c r="G4" s="1">
+        <v>1</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="1">
+        <v>1</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>1</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>1</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="1">
+        <v>1</v>
+      </c>
+      <c r="E8" s="1">
+        <v>1</v>
+      </c>
+      <c r="F8" s="1">
+        <v>1</v>
+      </c>
+      <c r="G8" s="1">
+        <v>1</v>
+      </c>
+      <c r="H8" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1">
+        <v>1</v>
+      </c>
+      <c r="F9" s="1">
+        <v>1</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E10" s="1">
+        <v>1</v>
+      </c>
+      <c r="F10" s="1">
+        <v>1</v>
+      </c>
+      <c r="G10" s="1">
+        <v>1</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="B11" s="1">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1">
+        <v>1</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11" s="1">
+        <v>1</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>1</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="1">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1">
+        <v>1</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1">
+        <v>1</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" s="1">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="1">
+        <v>1</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16" s="1">
+        <v>1</v>
+      </c>
+      <c r="F16" s="1">
+        <v>1</v>
+      </c>
+      <c r="G16" s="1">
+        <v>1</v>
+      </c>
+      <c r="H16" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>1</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G18" s="1">
+        <v>1</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1">
+        <v>1</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C20" s="1">
+        <v>1</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1">
+        <v>1</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1</v>
+      </c>
+      <c r="G20" s="1">
+        <v>1</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="1">
+        <v>1</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="1">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1">
+        <v>1</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B22" s="1">
+        <v>1</v>
+      </c>
+      <c r="C22" s="1">
+        <v>1</v>
+      </c>
+      <c r="D22" s="1">
+        <v>1</v>
+      </c>
+      <c r="E22" s="1">
+        <v>1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>1</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="1">
+        <v>1</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1</v>
+      </c>
+      <c r="C24" s="1">
+        <v>1</v>
+      </c>
+      <c r="D24" s="1">
+        <v>1</v>
+      </c>
+      <c r="E24" s="1">
+        <v>1</v>
+      </c>
+      <c r="F24" s="1">
+        <v>1</v>
+      </c>
+      <c r="G24" s="1">
+        <v>1</v>
+      </c>
+      <c r="H24" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="1">
+        <v>1</v>
+      </c>
+      <c r="C25" s="1">
+        <v>1</v>
+      </c>
+      <c r="D25" s="1">
+        <v>1</v>
+      </c>
+      <c r="E25" s="1">
+        <v>1</v>
+      </c>
+      <c r="F25" s="1">
+        <v>1</v>
+      </c>
+      <c r="G25" s="1">
+        <v>1</v>
+      </c>
+      <c r="H25" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix for #7 #8
Not tag in when immobilizer activated
No ignition on at the second time without a reboot(removed 1 sec timer stop from ign off
</commit_message>
<xml_diff>
--- a/HEMSv1.1 Configs/Version control.xlsx
+++ b/HEMSv1.1 Configs/Version control.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="39">
   <si>
     <t>Powerloss/Restore logic for all assets</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>Remove Power disconnect</t>
+  </si>
+  <si>
+    <t>remove 1 second timer stop from Ignition logic</t>
+  </si>
+  <si>
+    <t>No tag in when immobilizer activated, remove timer7 at tag</t>
+  </si>
+  <si>
+    <t>add timer6 along with Tag in</t>
   </si>
 </sst>
 </file>
@@ -466,10 +475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1112,24 +1121,8 @@
       <c r="B25" s="1">
         <v>1</v>
       </c>
-      <c r="C25" s="1">
-        <v>1</v>
-      </c>
-      <c r="D25" s="1">
-        <v>1</v>
-      </c>
-      <c r="E25" s="1">
-        <v>1</v>
-      </c>
-      <c r="F25" s="1">
-        <v>1</v>
-      </c>
-      <c r="G25" s="1">
-        <v>1</v>
-      </c>
-      <c r="H25" s="1">
-        <v>1</v>
-      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
@@ -1159,6 +1152,84 @@
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1</v>
+      </c>
+      <c r="E27" s="1">
+        <v>1</v>
+      </c>
+      <c r="F27" s="1">
+        <v>1</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B28" s="1">
+        <v>1</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="1">
+        <v>1</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="1">
+        <v>1</v>
+      </c>
+      <c r="H29" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Deleted 1 second timer protection
Delete 1 second timer protection
</commit_message>
<xml_diff>
--- a/HEMSv1.1 Configs/Version control.xlsx
+++ b/HEMSv1.1 Configs/Version control.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="139">
   <si>
     <t>Powerloss/Restore logic for all assets</t>
   </si>
@@ -432,9 +432,6 @@
   </si>
   <si>
     <t>$PFAL,CNF.Set,AL99</t>
-  </si>
-  <si>
-    <t>Add 1 second timer protection</t>
   </si>
 </sst>
 </file>
@@ -779,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,13 +1531,6 @@
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>